<commit_message>
FM_disturber: update coil inductance formula
</commit_message>
<xml_diff>
--- a/Projects/FM_Disturber/01-Simulation/Calculation.xlsx
+++ b/Projects/FM_Disturber/01-Simulation/Calculation.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>2N3904</t>
   </si>
@@ -144,10 +144,16 @@
     <t>d</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>n</t>
+    <t>D</t>
+  </si>
+  <si>
+    <t>ur</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>length</t>
   </si>
 </sst>
 </file>
@@ -251,14 +257,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -267,6 +270,10 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -369,20 +376,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>476940</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>124117</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>734660</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>124512</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Grafik 2"/>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -395,8 +402,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4752975" y="4381500"/>
-          <a:ext cx="4944165" cy="2095792"/>
+          <a:off x="5295900" y="2638425"/>
+          <a:ext cx="8849960" cy="4925112"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -652,10 +659,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -680,10 +687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -915,34 +922,34 @@
     </row>
     <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="6"/>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="7">
         <f>B33/2</f>
         <v>1.2181775118586704E-7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="7">
         <f>1/((2*PI()*B17)^2*B34)</f>
         <v>2.4363550237173409E-7</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="9">
         <v>1.7999999999999999E-11</v>
       </c>
       <c r="C34" t="s">
@@ -952,29 +959,53 @@
         <v>37</v>
       </c>
     </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37" s="2">
-        <v>0.05</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="2">
-        <v>0.01</v>
+        <v>4.0000000000000002E-4</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>40</v>
       </c>
-      <c r="B39">
-        <f>SQRT(B32*1000000*(18*B37/25.4+40*B38/25.4)/((B37/25.4)^2))</f>
-        <v>40.111954049421868</v>
+      <c r="B40" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <f>SQRT(B36*B39/(B40*0.00000126*PI()*B37^2/4))</f>
+        <v>11.192387328628595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
blog: add new pictures
</commit_message>
<xml_diff>
--- a/Projects/FM_Disturber/01-Simulation/Calculation.xlsx
+++ b/Projects/FM_Disturber/01-Simulation/Calculation.xlsx
@@ -1,23 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vtolentino\Documents\test\Kicad\Projects\FM_Disturber\01-Simulation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2N3904_Characteristic" sheetId="1" r:id="rId1"/>
     <sheet name="Calculation" sheetId="2" r:id="rId2"/>
+    <sheet name="Calculation_new" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
   <si>
     <t>2N3904</t>
   </si>
@@ -157,13 +153,16 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,7 +278,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -376,6 +375,49 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>734660</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>124512</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5295900" y="2638425"/>
+          <a:ext cx="8849960" cy="4925112"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -642,32 +684,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Design1" id="{1AD34F71-B67C-4BDB-AA9C-810616DF2371}" vid="{AADBB762-B76A-4E46-AF1D-B465C5AAA2F0}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Design1" id="{1AD34F71-B67C-4BDB-AA9C-810616DF2371}" vid="{AADBB762-B76A-4E46-AF1D-B465C5AAA2F0}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -689,16 +731,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
@@ -706,7 +748,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -723,7 +765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -744,7 +786,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -758,7 +800,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -767,7 +809,7 @@
         <v>0.47156666666666663</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -776,7 +818,7 @@
         <v>3.3333333333333333E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -785,7 +827,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -793,7 +835,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -802,7 +844,7 @@
         <v>563530</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -814,7 +856,7 @@
         <v>5600</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -822,7 +864,7 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -831,7 +873,7 @@
         <v>1.1215666666666666</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -840,7 +882,7 @@
         <v>336470</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -848,7 +890,7 @@
         <v>76000000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -857,7 +899,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -869,7 +911,7 @@
         <v>4.6999999999999999E-11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -880,7 +922,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -892,12 +934,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -906,7 +948,7 @@
         <v>8.7708780853824262E-11</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -915,7 +957,7 @@
         <v>4.3854390426912131E-11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -923,14 +965,14 @@
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15" thickBot="1"/>
+    <row r="31" spans="1:3">
       <c r="A31" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="5"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" s="6" t="s">
         <v>35</v>
       </c>
@@ -939,7 +981,7 @@
         <v>1.2181775118586704E-7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" s="6" t="s">
         <v>34</v>
       </c>
@@ -948,7 +990,7 @@
         <v>2.4363550237173409E-7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15" thickBot="1">
       <c r="A34" s="8" t="s">
         <v>33</v>
       </c>
@@ -962,7 +1004,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -970,7 +1012,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -978,7 +1020,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -986,7 +1028,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -994,7 +1036,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -1002,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1011,7 +1053,7 @@
         <v>11.192387328628595</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1019,7 +1061,7 @@
         <v>1.5E-11</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>33</v>
       </c>
@@ -1028,7 +1070,7 @@
         <v>7.5E-12</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>30</v>
       </c>
@@ -1036,7 +1078,383 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="2">
+        <f>1/(2*PI()*SQRT(B45*B46))</f>
+        <v>58115168.313254729</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <f>B2/2</f>
+        <v>1.5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>300</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <f>(B4+B6)*B9</f>
+        <v>0.24079999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <f>B4/F3</f>
+        <v>3.3333333333333333E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <f>(B2-B3)/B4</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <f>(B2-F4-B5)/B6</f>
+        <v>632760</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <f>B12*B15/(B12+B15)*(B2/B14-1)</f>
+        <v>9101.4383713210882</v>
+      </c>
+      <c r="C11" s="2">
+        <v>9100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <f>F4+B5</f>
+        <v>0.89080000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2">
+        <f>B14/B6</f>
+        <v>267240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2">
+        <v>76000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <f>B9/10</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2">
+        <f>1/(2*PI()*B17*B18)</f>
+        <v>8.7255999502135611E-11</v>
+      </c>
+      <c r="C19" s="2">
+        <v>4.6999999999999999E-11</v>
+      </c>
+      <c r="E19">
+        <f>B14*B11/(B2-B14)</f>
+        <v>3843.9035184775394</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <f>B14*B11/(B2-B14)</f>
+        <v>3843.9035184775394</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="2">
+        <f>B15*B11/(B15+B11)</f>
+        <v>8801.6781148963946</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="2">
+        <f>1/(2*PI()*B17*B21/100)</f>
+        <v>5.4479618907830581E-11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2">
+        <f>B27*2</f>
+        <v>8.7708780853824262E-11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="2">
+        <f>1/((2*PI()*B17)^2*B28)</f>
+        <v>4.3854390426912131E-11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickBot="1"/>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="7">
+        <f>B33/2</f>
+        <v>1.2181775118586704E-7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="7">
+        <f>1/((2*PI()*B17)^2*B34)</f>
+        <v>2.4363550237173409E-7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" thickBot="1">
+      <c r="A34" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9">
+        <v>1.7999999999999999E-11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="2">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <f>SQRT(B36*B39/(B40*0.00000126*PI()*B37^2/4))</f>
+        <v>11.192387328628595</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1.5E-11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="2">
+        <f>B44/2</f>
+        <v>7.5E-12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>43</v>
       </c>

</xml_diff>